<commit_message>
Additional test cases with Pass/Fail formatting
</commit_message>
<xml_diff>
--- a/Group 4 Test Cases.xlsx
+++ b/Group 4 Test Cases.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="86">
   <si>
     <t>User Test Cases</t>
   </si>
@@ -252,13 +252,37 @@
   </si>
   <si>
     <t>Item is not checked out to user</t>
+  </si>
+  <si>
+    <t>Item RenewalTest Cases</t>
+  </si>
+  <si>
+    <t>Renew Item Validation</t>
+  </si>
+  <si>
+    <t>Find the name of a non-overdue book to return and click the "Renew Item" button</t>
+  </si>
+  <si>
+    <t>No More Renewals Validation</t>
+  </si>
+  <si>
+    <t>Find a book the user has already renewed</t>
+  </si>
+  <si>
+    <t>Item found</t>
+  </si>
+  <si>
+    <t>Verify the "Renew Item" button is disabled.</t>
+  </si>
+  <si>
+    <t>Button disabled, user unable to renew item.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+  <fonts count="8">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -278,13 +302,42 @@
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12.0"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12.0"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <color rgb="FF000000"/>
+      <name val="Inconsolata"/>
+    </font>
+    <font>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="5">
@@ -337,7 +390,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="16">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -352,18 +405,27 @@
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" readingOrder="0"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="4" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right" readingOrder="0"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="4" fillId="2" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
+    <xf borderId="0" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="4" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="0" fillId="2" fontId="6" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -656,9 +718,10 @@
         <v>2</v>
       </c>
       <c r="D3" s="8" t="str">
-        <f>if(AND(D4="PASS",D5="PASS",D6="PASS",D7="PASS",D8="PASS",D9="PASS",D11="PASS"),"PASS","FAIL")</f>
-        <v>PASS</v>
-      </c>
+        <f>if(or(ISBLANK(D4),ISBLANK(D5),isblank(D6),isblank(D7),isblank(D8),isblank(D9),isblank(D10),isblank(D11)),"incomplete",if(AND(D4="PASS",D5="PASS",D6="PASS",D7="PASS",D8="PASS",D9="PASS",D10="PASS",D11="PASS"),"PASS","FAIL"))</f>
+        <v>incomplete</v>
+      </c>
+      <c r="H3" s="9"/>
     </row>
     <row r="4">
       <c r="A4" s="4">
@@ -670,7 +733,8 @@
       <c r="C4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="10"/>
+      <c r="E4" s="4" t="s">
         <v>5</v>
       </c>
     </row>
@@ -684,9 +748,7 @@
       <c r="C5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="4" t="s">
-        <v>5</v>
-      </c>
+      <c r="D5" s="10"/>
     </row>
     <row r="6">
       <c r="A6" s="4">
@@ -698,9 +760,7 @@
       <c r="C6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="4" t="s">
-        <v>5</v>
-      </c>
+      <c r="D6" s="10"/>
     </row>
     <row r="7">
       <c r="A7" s="4">
@@ -712,9 +772,7 @@
       <c r="C7" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="4" t="s">
-        <v>5</v>
-      </c>
+      <c r="D7" s="10"/>
     </row>
     <row r="8">
       <c r="A8" s="4">
@@ -726,9 +784,7 @@
       <c r="C8" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="4" t="s">
-        <v>5</v>
-      </c>
+      <c r="D8" s="10"/>
     </row>
     <row r="9">
       <c r="A9" s="4">
@@ -740,9 +796,7 @@
       <c r="C9" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="4" t="s">
-        <v>5</v>
-      </c>
+      <c r="D9" s="10"/>
     </row>
     <row r="10">
       <c r="A10" s="4">
@@ -754,9 +808,7 @@
       <c r="C10" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="4" t="s">
-        <v>5</v>
-      </c>
+      <c r="D10" s="10"/>
     </row>
     <row r="11">
       <c r="A11" s="4">
@@ -768,21 +820,19 @@
       <c r="C11" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="4" t="s">
-        <v>5</v>
-      </c>
+      <c r="D11" s="10"/>
     </row>
     <row r="13">
-      <c r="A13" s="8" t="s">
+      <c r="A13" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="9"/>
+      <c r="B13" s="12"/>
       <c r="C13" s="7" t="s">
         <v>2</v>
       </c>
       <c r="D13" s="8" t="str">
-        <f>if(AND(D14="PASS",D15="PASS",D16="PASS",D17="PASS",D18="PASS",D19="PASS",D20="PASS",D21="PASS"),"PASS","FAIL")</f>
-        <v>PASS</v>
+        <f>if(or(ISBLANK(D14),ISBLANK(D15),isblank(D16),isblank(D17),isblank(D18),isblank(D19),isblank(D20),isblank(D21)),"incomplete",if(AND(D14="PASS",D15="PASS",D16="PASS",D17="PASS",D18="PASS",D19="PASS",D20="PASS",D21="PASS"),"PASS","FAIL"))</f>
+        <v>incomplete</v>
       </c>
     </row>
     <row r="14">
@@ -795,9 +845,8 @@
       <c r="C14" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D14" s="4" t="s">
-        <v>5</v>
-      </c>
+      <c r="D14" s="10"/>
+      <c r="E14" s="13"/>
     </row>
     <row r="15">
       <c r="A15" s="4">
@@ -809,9 +858,7 @@
       <c r="C15" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D15" s="4" t="s">
-        <v>5</v>
-      </c>
+      <c r="D15" s="10"/>
     </row>
     <row r="16">
       <c r="A16" s="4">
@@ -823,9 +870,7 @@
       <c r="C16" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D16" s="4" t="s">
-        <v>5</v>
-      </c>
+      <c r="D16" s="10"/>
     </row>
     <row r="17">
       <c r="A17" s="4">
@@ -837,9 +882,7 @@
       <c r="C17" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D17" s="4" t="s">
-        <v>5</v>
-      </c>
+      <c r="D17" s="10"/>
     </row>
     <row r="18">
       <c r="A18" s="4">
@@ -851,9 +894,7 @@
       <c r="C18" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D18" s="4" t="s">
-        <v>5</v>
-      </c>
+      <c r="D18" s="10"/>
     </row>
     <row r="19">
       <c r="A19" s="4">
@@ -865,9 +906,7 @@
       <c r="C19" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D19" s="4" t="s">
-        <v>5</v>
-      </c>
+      <c r="D19" s="10"/>
     </row>
     <row r="20">
       <c r="A20" s="4">
@@ -879,9 +918,7 @@
       <c r="C20" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D20" s="4" t="s">
-        <v>5</v>
-      </c>
+      <c r="D20" s="10"/>
     </row>
     <row r="21">
       <c r="A21" s="4">
@@ -893,9 +930,7 @@
       <c r="C21" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D21" s="4" t="s">
-        <v>5</v>
-      </c>
+      <c r="D21" s="10"/>
     </row>
     <row r="23">
       <c r="A23" s="6" t="s">
@@ -906,8 +941,8 @@
         <v>2</v>
       </c>
       <c r="D23" s="8" t="str">
-        <f>if(AND(D24="PASS",D25="PASS"),"PASS","FAIL")</f>
-        <v>PASS</v>
+        <f>if(or(ISBLANK(D24),ISBLANK(D25)),"incomplete",if(AND(D24="PASS",D25="PASS"),"PASS","FAIL"))</f>
+        <v>incomplete</v>
       </c>
     </row>
     <row r="24">
@@ -920,9 +955,7 @@
       <c r="C24" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D24" s="4" t="s">
-        <v>5</v>
-      </c>
+      <c r="D24" s="10"/>
     </row>
     <row r="25">
       <c r="A25" s="4">
@@ -934,15 +967,13 @@
       <c r="C25" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D25" s="4" t="s">
-        <v>5</v>
-      </c>
+      <c r="D25" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="3">
+    <mergeCell ref="A1:D1"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A1:D1"/>
   </mergeCells>
   <conditionalFormatting sqref="D3:D11 D13:D21 D23:D25">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
@@ -955,7 +986,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" sqref="D3:D11 D13:D21 D23:D25">
+    <dataValidation type="list" allowBlank="1" sqref="D4:D11 D14:D21 D24:D25">
       <formula1>"PASS,FAIL"</formula1>
     </dataValidation>
   </dataValidations>
@@ -976,7 +1007,7 @@
     <col customWidth="1" min="1" max="1" width="6.13"/>
     <col customWidth="1" min="2" max="2" width="36.63"/>
     <col customWidth="1" min="3" max="3" width="46.0"/>
-    <col customWidth="1" min="4" max="4" width="7.88"/>
+    <col customWidth="1" min="4" max="4" width="11.5"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1000,8 +1031,8 @@
         <v>2</v>
       </c>
       <c r="D3" s="8" t="str">
-        <f>if(AND(D4="PASS",D5="PASS",D6="PASS",D7="PASS",D8="PASS",D9="PASS"),"PASS","FAIL")</f>
-        <v>PASS</v>
+        <f>if(or(ISBLANK(D4),ISBLANK(D5),isblank(D6),isblank(D7),isblank(D8),isblank(D9)),"incomplete",if(AND(D4="PASS",D5="PASS",D6="PASS",D7="PASS",D8="PASS",D9="PASS"),"PASS","FAIL"))</f>
+        <v>incomplete</v>
       </c>
     </row>
     <row r="4">
@@ -1014,9 +1045,7 @@
       <c r="C4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>5</v>
-      </c>
+      <c r="D4" s="10"/>
     </row>
     <row r="5">
       <c r="A5" s="4">
@@ -1028,9 +1057,7 @@
       <c r="C5" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="4" t="s">
-        <v>5</v>
-      </c>
+      <c r="D5" s="10"/>
     </row>
     <row r="6">
       <c r="A6" s="4">
@@ -1042,9 +1069,7 @@
       <c r="C6" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D6" s="4" t="s">
-        <v>5</v>
-      </c>
+      <c r="D6" s="10"/>
     </row>
     <row r="7">
       <c r="A7" s="4">
@@ -1056,9 +1081,7 @@
       <c r="C7" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D7" s="4" t="s">
-        <v>5</v>
-      </c>
+      <c r="D7" s="10"/>
     </row>
     <row r="8">
       <c r="A8" s="4">
@@ -1070,9 +1093,7 @@
       <c r="C8" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D8" s="4" t="s">
-        <v>5</v>
-      </c>
+      <c r="D8" s="10"/>
     </row>
     <row r="9">
       <c r="A9" s="4">
@@ -1084,9 +1105,7 @@
       <c r="C9" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D9" s="4" t="s">
-        <v>5</v>
-      </c>
+      <c r="D9" s="10"/>
     </row>
     <row r="11">
       <c r="A11" s="6" t="s">
@@ -1097,8 +1116,8 @@
         <v>2</v>
       </c>
       <c r="D11" s="8" t="str">
-        <f>if(AND(D12="PASS",D13="PASS",D14="PASS",D15="PASS",D16="PASS",D17="PASS"),"PASS","FAIL")</f>
-        <v>PASS</v>
+        <f>if(or(ISBLANK(D12),ISBLANK(D13),isblank(D14),isblank(D15),isblank(D16),isblank(D17),isblank(D18),isblank(D19),isblank(D20)),"incomplete",if(AND(D12="PASS",D13="PASS",D14="PASS",D15="PASS",D16="PASS",D17="PASS",D18="PASS",D19="PASS",D20="PASS"),"PASS","FAIL"))</f>
+        <v>incomplete</v>
       </c>
     </row>
     <row r="12">
@@ -1111,9 +1130,7 @@
       <c r="C12" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D12" s="4" t="s">
-        <v>5</v>
-      </c>
+      <c r="D12" s="10"/>
     </row>
     <row r="13">
       <c r="A13" s="4">
@@ -1125,9 +1142,7 @@
       <c r="C13" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D13" s="4" t="s">
-        <v>5</v>
-      </c>
+      <c r="D13" s="10"/>
     </row>
     <row r="14">
       <c r="A14" s="4">
@@ -1139,9 +1154,7 @@
       <c r="C14" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D14" s="4" t="s">
-        <v>5</v>
-      </c>
+      <c r="D14" s="10"/>
     </row>
     <row r="15">
       <c r="A15" s="4">
@@ -1153,9 +1166,7 @@
       <c r="C15" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D15" s="4" t="s">
-        <v>5</v>
-      </c>
+      <c r="D15" s="10"/>
     </row>
     <row r="16">
       <c r="A16" s="4">
@@ -1167,9 +1178,7 @@
       <c r="C16" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D16" s="4" t="s">
-        <v>5</v>
-      </c>
+      <c r="D16" s="10"/>
     </row>
     <row r="17">
       <c r="A17" s="4">
@@ -1181,9 +1190,7 @@
       <c r="C17" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D17" s="4" t="s">
-        <v>5</v>
-      </c>
+      <c r="D17" s="10"/>
     </row>
     <row r="18">
       <c r="A18" s="4">
@@ -1195,9 +1202,7 @@
       <c r="C18" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D18" s="4" t="s">
-        <v>5</v>
-      </c>
+      <c r="D18" s="10"/>
     </row>
     <row r="19">
       <c r="A19" s="4">
@@ -1209,9 +1214,7 @@
       <c r="C19" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D19" s="4" t="s">
-        <v>5</v>
-      </c>
+      <c r="D19" s="10"/>
     </row>
     <row r="20">
       <c r="A20" s="4">
@@ -1223,15 +1226,13 @@
       <c r="C20" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="D20" s="4" t="s">
-        <v>5</v>
-      </c>
+      <c r="D20" s="10"/>
     </row>
     <row r="21">
-      <c r="A21" s="10"/>
-      <c r="B21" s="10"/>
-      <c r="C21" s="10"/>
-      <c r="D21" s="10"/>
+      <c r="A21" s="14"/>
+      <c r="B21" s="14"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="14"/>
     </row>
     <row r="22">
       <c r="A22" s="6" t="s">
@@ -1242,8 +1243,8 @@
         <v>2</v>
       </c>
       <c r="D22" s="8" t="str">
-        <f>if(AND(D23="PASS",D24="PASS",D25="PASS"),"PASS","FAIL")</f>
-        <v>PASS</v>
+        <f>if(or(ISBLANK(D23),ISBLANK(D24),isblank(D25)),"incomplete",if(AND(D23="PASS",D24="PASS",D25="PASS"),"PASS","FAIL"))</f>
+        <v>incomplete</v>
       </c>
     </row>
     <row r="23">
@@ -1256,9 +1257,7 @@
       <c r="C23" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D23" s="4" t="s">
-        <v>5</v>
-      </c>
+      <c r="D23" s="10"/>
     </row>
     <row r="24">
       <c r="A24" s="4">
@@ -1270,9 +1269,7 @@
       <c r="C24" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="D24" s="4" t="s">
-        <v>5</v>
-      </c>
+      <c r="D24" s="10"/>
     </row>
     <row r="25">
       <c r="A25" s="4">
@@ -1284,16 +1281,14 @@
       <c r="C25" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D25" s="4" t="s">
-        <v>5</v>
-      </c>
+      <c r="D25" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="4">
+    <mergeCell ref="A1:D1"/>
     <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A11:B11"/>
     <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A11:B11"/>
   </mergeCells>
   <conditionalFormatting sqref="D3:D9 D11:D20 D22:D25">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
@@ -1306,7 +1301,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" sqref="D3:D9 D11:D20 D22:D25">
+    <dataValidation type="list" allowBlank="1" sqref="D4:D9 D12:D20 D23:D25">
       <formula1>"PASS,FAIL"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1327,7 +1322,7 @@
     <col customWidth="1" min="1" max="1" width="5.13"/>
     <col customWidth="1" min="2" max="2" width="64.5"/>
     <col customWidth="1" min="3" max="3" width="46.0"/>
-    <col customWidth="1" min="4" max="4" width="7.88"/>
+    <col customWidth="1" min="4" max="4" width="11.5"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1351,8 +1346,8 @@
         <v>2</v>
       </c>
       <c r="D3" s="8" t="str">
-        <f>if(AND(D4="PASS",D5="PASS"),"PASS","FAIL")</f>
-        <v>PASS</v>
+        <f>if(or(ISBLANK(D4),ISBLANK(D5)),"incomplete",if(AND(D4="PASS",D5="PASS"),"PASS","FAIL"))</f>
+        <v>incomplete</v>
       </c>
     </row>
     <row r="4">
@@ -1365,9 +1360,7 @@
       <c r="C4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>5</v>
-      </c>
+      <c r="D4" s="10"/>
     </row>
     <row r="5">
       <c r="A5" s="4">
@@ -1379,9 +1372,7 @@
       <c r="C5" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="D5" s="4" t="s">
-        <v>5</v>
-      </c>
+      <c r="D5" s="10"/>
     </row>
     <row r="7">
       <c r="A7" s="6" t="s">
@@ -1392,8 +1383,8 @@
         <v>2</v>
       </c>
       <c r="D7" s="8" t="str">
-        <f>if(AND(D8="PASS",D9="PASS",D10="PASS",D11="PASS"),"PASS","FAIL")</f>
-        <v>PASS</v>
+        <f>if(or(ISBLANK(D8),ISBLANK(D9),isblank(D10),isblank(D11)),"incomplete",if(AND(D8="PASS",D9="PASS",D10="PASS",D11="PASS"),"PASS","FAIL"))</f>
+        <v>incomplete</v>
       </c>
     </row>
     <row r="8">
@@ -1406,9 +1397,7 @@
       <c r="C8" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="4" t="s">
-        <v>5</v>
-      </c>
+      <c r="D8" s="10"/>
     </row>
     <row r="9">
       <c r="A9" s="4">
@@ -1420,9 +1409,7 @@
       <c r="C9" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="D9" s="4" t="s">
-        <v>5</v>
-      </c>
+      <c r="D9" s="10"/>
     </row>
     <row r="10">
       <c r="A10" s="4">
@@ -1434,9 +1421,7 @@
       <c r="C10" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="D10" s="4" t="s">
-        <v>5</v>
-      </c>
+      <c r="D10" s="10"/>
     </row>
     <row r="11">
       <c r="A11" s="4">
@@ -1448,9 +1433,7 @@
       <c r="C11" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="D11" s="4" t="s">
-        <v>5</v>
-      </c>
+      <c r="D11" s="10"/>
     </row>
     <row r="13">
       <c r="A13" s="6" t="s">
@@ -1461,8 +1444,8 @@
         <v>2</v>
       </c>
       <c r="D13" s="8" t="str">
-        <f>if(AND(D14="PASS",D15="PASS",D16="PASS"),"PASS","FAIL")</f>
-        <v>PASS</v>
+        <f>if(or(ISBLANK(D14),ISBLANK(D15),isblank(D16)),"incomplete",if(AND(D14="PASS",D15="PASS",D16="PASS"),"PASS","FAIL"))</f>
+        <v>incomplete</v>
       </c>
     </row>
     <row r="14">
@@ -1475,9 +1458,7 @@
       <c r="C14" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D14" s="4" t="s">
-        <v>5</v>
-      </c>
+      <c r="D14" s="10"/>
     </row>
     <row r="15">
       <c r="A15" s="4">
@@ -1489,9 +1470,7 @@
       <c r="C15" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="D15" s="4" t="s">
-        <v>5</v>
-      </c>
+      <c r="D15" s="10"/>
     </row>
     <row r="16">
       <c r="A16" s="4">
@@ -1503,14 +1482,12 @@
       <c r="C16" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D16" s="4" t="s">
-        <v>5</v>
-      </c>
+      <c r="D16" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="4">
+    <mergeCell ref="A1:D1"/>
     <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A1:D1"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A13:B13"/>
   </mergeCells>
@@ -1525,7 +1502,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" sqref="D3:D5 D7:D11 D13:D16">
+    <dataValidation type="list" allowBlank="1" sqref="D4:D5 D8:D11 D14:D16">
       <formula1>"PASS,FAIL"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1546,7 +1523,7 @@
     <col customWidth="1" min="1" max="1" width="5.0"/>
     <col customWidth="1" min="2" max="2" width="45.88"/>
     <col customWidth="1" min="3" max="3" width="46.0"/>
-    <col customWidth="1" min="4" max="4" width="7.88"/>
+    <col customWidth="1" min="4" max="4" width="11.5"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1570,8 +1547,8 @@
         <v>2</v>
       </c>
       <c r="D3" s="8" t="str">
-        <f>if(AND(D4="PASS",D5="PASS",D6="PASS",D7="PASS",#REF!="PASS",#REF!="PASS"),"PASS","FAIL")</f>
-        <v>#REF!</v>
+        <f>if(or(ISBLANK(D4),ISBLANK(D5),isblank(D6),isblank(D7)),"incomplete",if(AND(D4="PASS",D5="PASS",D6="PASS",D7="PASS"),"PASS","FAIL"))</f>
+        <v>incomplete</v>
       </c>
     </row>
     <row r="4">
@@ -1584,9 +1561,7 @@
       <c r="C4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>5</v>
-      </c>
+      <c r="D4" s="10"/>
     </row>
     <row r="5">
       <c r="A5" s="4">
@@ -1598,9 +1573,7 @@
       <c r="C5" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="D5" s="4" t="s">
-        <v>5</v>
-      </c>
+      <c r="D5" s="10"/>
     </row>
     <row r="6">
       <c r="A6" s="4">
@@ -1612,9 +1585,7 @@
       <c r="C6" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="D6" s="4" t="s">
-        <v>5</v>
-      </c>
+      <c r="D6" s="10"/>
     </row>
     <row r="7">
       <c r="A7" s="4">
@@ -1626,9 +1597,7 @@
       <c r="C7" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="D7" s="4" t="s">
-        <v>5</v>
-      </c>
+      <c r="D7" s="10"/>
     </row>
     <row r="9">
       <c r="A9" s="6" t="s">
@@ -1639,8 +1608,8 @@
         <v>2</v>
       </c>
       <c r="D9" s="8" t="str">
-        <f>if(AND(D10="PASS",D11="PASS",D12="PASS",#REF!="PASS",#REF!="PASS",#REF!="PASS"),"PASS","FAIL")</f>
-        <v>#REF!</v>
+        <f>if(or(ISBLANK(D10),ISBLANK(D11),isblank(D12)),"incomplete",if(AND(D10="PASS",D11="PASS",D12="PASS"),"PASS","FAIL"))</f>
+        <v>incomplete</v>
       </c>
     </row>
     <row r="10">
@@ -1653,9 +1622,7 @@
       <c r="C10" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="4" t="s">
-        <v>5</v>
-      </c>
+      <c r="D10" s="10"/>
     </row>
     <row r="11">
       <c r="A11" s="4">
@@ -1667,9 +1634,7 @@
       <c r="C11" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="D11" s="4" t="s">
-        <v>5</v>
-      </c>
+      <c r="D11" s="10"/>
     </row>
     <row r="12">
       <c r="A12" s="4">
@@ -1681,9 +1646,7 @@
       <c r="C12" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="D12" s="4" t="s">
-        <v>5</v>
-      </c>
+      <c r="D12" s="10"/>
     </row>
     <row r="14">
       <c r="A14" s="6" t="s">
@@ -1694,8 +1657,8 @@
         <v>2</v>
       </c>
       <c r="D14" s="8" t="str">
-        <f>if(AND(D15="PASS",D16="PASS",D17="PASS",D18="PASS"),"PASS","FAIL")</f>
-        <v>PASS</v>
+        <f>if(or(ISBLANK(D15),ISBLANK(D16),isblank(D17),isblank(D18)),"incomplete",if(AND(D15="PASS",D16="PASS",D17="PASS",D18="PASS"),"PASS","FAIL"))</f>
+        <v>incomplete</v>
       </c>
     </row>
     <row r="15">
@@ -1708,9 +1671,7 @@
       <c r="C15" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D15" s="4" t="s">
-        <v>5</v>
-      </c>
+      <c r="D15" s="10"/>
     </row>
     <row r="16">
       <c r="A16" s="4">
@@ -1722,9 +1683,7 @@
       <c r="C16" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="D16" s="4" t="s">
-        <v>5</v>
-      </c>
+      <c r="D16" s="10"/>
     </row>
     <row r="17">
       <c r="A17" s="4">
@@ -1736,9 +1695,7 @@
       <c r="C17" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="D17" s="4" t="s">
-        <v>5</v>
-      </c>
+      <c r="D17" s="10"/>
     </row>
     <row r="18">
       <c r="A18" s="4">
@@ -1750,15 +1707,13 @@
       <c r="C18" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="D18" s="4" t="s">
-        <v>5</v>
-      </c>
+      <c r="D18" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="4">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A3:B3"/>
     <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A1:D1"/>
     <mergeCell ref="A14:B14"/>
   </mergeCells>
   <conditionalFormatting sqref="D3:D7 D9:D12 D14:D18">
@@ -1772,7 +1727,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" sqref="D3:D7 D9:D12 D14:D18">
+    <dataValidation type="list" allowBlank="1" sqref="D4:D7 D10:D12 D15:D18">
       <formula1>"PASS,FAIL"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1789,7 +1744,127 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
-  <sheetData/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="5.13"/>
+    <col customWidth="1" min="2" max="2" width="60.88"/>
+    <col customWidth="1" min="3" max="3" width="46.0"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="3"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="8" t="str">
+        <f>if(or(ISBLANK(D4),ISBLANK(D5)),"incomplete",if(AND(D4="PASS",D5="PASS"),"PASS","FAIL"))</f>
+        <v>incomplete</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="10"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" s="10"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B7" s="3"/>
+      <c r="C7" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="8" t="str">
+        <f>if(or(ISBLANK(D8),ISBLANK(D9),isblank(D10)),"incomplete",if(AND(D8="PASS",D9="PASS",D10="PASS"),"PASS","FAIL"))</f>
+        <v>incomplete</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="10"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D9" s="10"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D10" s="10"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A7:B7"/>
+  </mergeCells>
+  <conditionalFormatting sqref="D3:D5 D7:D10">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>"PASS"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D3:D5 D7:D10">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+      <formula>"FAIL"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations>
+    <dataValidation type="list" allowBlank="1" sqref="D4:D5 D8:D10">
+      <formula1>"PASS,FAIL"</formula1>
+    </dataValidation>
+  </dataValidations>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>

</xml_diff>